<commit_message>
Kafka: basic course 1.5/2
</commit_message>
<xml_diff>
--- a/202304_Kafka/202304_Kafka.xlsx
+++ b/202304_Kafka/202304_Kafka.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\202304_Kafka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F8B53D-60CA-47E1-9871-872A2B4CDF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF507B5A-46AB-47A4-A683-D2C9B43868D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4455" windowWidth="25440" windowHeight="15390" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
     <sheet name="S1" sheetId="2" r:id="rId2"/>
     <sheet name="S2-S4" sheetId="4" r:id="rId3"/>
-    <sheet name="S5" sheetId="5" r:id="rId4"/>
+    <sheet name="S5.Kafka" sheetId="5" r:id="rId4"/>
     <sheet name="S6" sheetId="6" r:id="rId5"/>
     <sheet name="S7" sheetId="7" r:id="rId6"/>
     <sheet name="S8" sheetId="8" r:id="rId7"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="535">
   <si>
     <t>https://www.udemy.com/course/apache_kafka/</t>
   </si>
@@ -1291,12 +1291,6 @@
     <t>S10</t>
   </si>
   <si>
-    <t>Topic; Message; Partitions; Partition Leader and Followers;</t>
-  </si>
-  <si>
-    <t>Controller;</t>
-  </si>
-  <si>
     <t>Create topic with multiple partitions</t>
   </si>
   <si>
@@ -1658,9 +1652,6 @@
     <t>=&gt; 3 x 7 = 21 partitions created. Each broker contains at least 7 partitions.</t>
   </si>
   <si>
-    <t>=&gt; Only Leader broker in the partition serves producers and consumers.</t>
-  </si>
-  <si>
     <t>Remains are just synchronize with Leader.</t>
   </si>
   <si>
@@ -1833,13 +1824,454 @@
   </si>
   <si>
     <t>some consumers will be idle and not receive msg at all.</t>
+  </si>
+  <si>
+    <t>server0.properties; server1.properties; server2.properties;</t>
+  </si>
+  <si>
+    <t>=&gt; Only Leader partition in the broker serves producers and consumers.</t>
+  </si>
+  <si>
+    <t>Topic name is unique across Cluster.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Offset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> number assigned to every messages.</t>
+    </r>
+  </si>
+  <si>
+    <t>New message appended after existing messages.</t>
+  </si>
+  <si>
+    <t>Messages could be deleted automatically if retention period has expired.</t>
+  </si>
+  <si>
+    <t>Message structure</t>
+  </si>
+  <si>
+    <t>unique across PARTITION.</t>
+  </si>
+  <si>
+    <t>Message should be as small as possible.</t>
+  </si>
+  <si>
+    <t>Topic &amp; Partition</t>
+  </si>
+  <si>
+    <t>How topics are stored on Brokers?</t>
+  </si>
+  <si>
+    <t>Topic A: 2 partitions</t>
+  </si>
+  <si>
+    <t>NOTE: Multiple partitions in the same topic may exist on the same broker.</t>
+  </si>
+  <si>
+    <t>E.g., Topic D</t>
+  </si>
+  <si>
+    <t>Topic B: 3 partitions</t>
+  </si>
+  <si>
+    <t>Topic D: 2 partitions</t>
+  </si>
+  <si>
+    <t>Topic C: 1 partition</t>
+  </si>
+  <si>
+    <t>Spreading messages across partitions</t>
+  </si>
+  <si>
+    <t>Kafka creates partitions starting from number Zero.</t>
+  </si>
+  <si>
+    <t>E.g., topic A: partition 0, partition 1</t>
+  </si>
+  <si>
+    <t>Offset number is unique for each partition, starts from 0.</t>
+  </si>
+  <si>
+    <t>Producers may write messages to different partitions.</t>
+  </si>
+  <si>
+    <t>What if a broker fails?</t>
+  </si>
+  <si>
+    <t>Partition inside broker will be disappear.</t>
+  </si>
+  <si>
+    <t>Those messages will simple be lost.</t>
+  </si>
+  <si>
+    <t>=&gt; Replicate messages inside of every partition!</t>
+  </si>
+  <si>
+    <t>=&gt; REPLICATION_FACTOR</t>
+  </si>
+  <si>
+    <t>Topic; Message; Partitions; REPLICATION - Partition Leader and Followers;</t>
+  </si>
+  <si>
+    <t>REPLICATION: Leader and Followers</t>
+  </si>
+  <si>
+    <t>Followers: get new messages from Leader and write to specific partition.</t>
+  </si>
+  <si>
+    <t>Don't serve producers/consumers</t>
+  </si>
+  <si>
+    <t>Leader: Server read/write operations.</t>
+  </si>
+  <si>
+    <t>If the Leader is down, either one of Followers will be the Leader.</t>
+  </si>
+  <si>
+    <t>Controllers</t>
+  </si>
+  <si>
+    <t>Who decides which broker will be the leader of partition?</t>
+  </si>
+  <si>
+    <t>Why broker 1 is the leader, broker 0 and broker 2 are followers?</t>
+  </si>
+  <si>
+    <t>Why partitions spread across brokers instead of all-in-one broker?</t>
+  </si>
+  <si>
+    <t>If broker 1 fails, where to move the partition 1?</t>
+  </si>
+  <si>
+    <t>-&gt; administrative tasks -&gt; Not Zookeeper.</t>
+  </si>
+  <si>
+    <t>Zookeeper elects the Controller from brokers.</t>
+  </si>
+  <si>
+    <t>-&gt; Controller is one active Broker.</t>
+  </si>
+  <si>
+    <t>How Producers write messages to Kafka?</t>
+  </si>
+  <si>
+    <t>Messages can be added spread across partitions or only a specific partition.</t>
+  </si>
+  <si>
+    <t>How Consumers read messages from topic?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normally consumer connects just to one topic. </t>
+  </si>
+  <si>
+    <t>But consumer can connect to multitple topics.</t>
+  </si>
+  <si>
+    <t>Consumer can consume messages either from all partitions or just one partition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiple consumers can consume messages from a single topic. </t>
+  </si>
+  <si>
+    <t>-&gt; consumer group.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a single message may </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>be consumed only by one</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of the consumer in group.</t>
+    </r>
+  </si>
+  <si>
+    <t>Consumer can consume messages from beginning, or only new messages,</t>
+  </si>
+  <si>
+    <t>or from a specific offset.</t>
+  </si>
+  <si>
+    <t>Controller; Producer; Consumer;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">--bootstrap-server </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>localhost:9092</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> \</t>
+    </r>
+  </si>
+  <si>
+    <t>--topic numbers</t>
+  </si>
+  <si>
+    <t>produce some messages: 1, 2, 3</t>
+  </si>
+  <si>
+    <t>START OTHER CONSOLE CONSUMER</t>
+  </si>
+  <si>
+    <t>If there is some topics with multiple producers who send messages to it at the very high rates,</t>
+  </si>
+  <si>
+    <t>single consumer may not be able to consume all produced messages at the same high rates.</t>
+  </si>
+  <si>
+    <t>=&gt; consumers may be organized into consumer groups to share consumption of the messages.</t>
+  </si>
+  <si>
+    <t>=&gt; reduce the loads of consumers.</t>
+  </si>
+  <si>
+    <t>=&gt; We see which consumer is consuming message from which partition.</t>
+  </si>
+  <si>
+    <t>Starting consumer in the custom consumer group</t>
+  </si>
+  <si>
+    <t>--topic numbers \</t>
+  </si>
+  <si>
+    <t>CURRENT-OFFSET = commited offsets (last offset received by consumer)</t>
+  </si>
+  <si>
+    <t>LOG-END-OFFSET = Last offset of the messages in the partition</t>
+  </si>
+  <si>
+    <t>LAG = LOG-END-OFFSET - CURRENT-OFFSET</t>
+  </si>
+  <si>
+    <t>Starting second consumer in the same consumer group</t>
+  </si>
+  <si>
+    <t>LAG &gt; 0 means consumer has not yet consumed all messages in the partition.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">=&gt; A single consumer group created: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>console-consumer-35655</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">=&gt; New consumer group created: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>console-consumer-35655, console-consumer-23234</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">--group </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>console-consumer-35655</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> \</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">--group </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>console-consumer-35655</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> \</t>
+    </r>
+  </si>
+  <si>
+    <t>Send some messages from producer</t>
+  </si>
+  <si>
+    <t>=&gt; Only one consumer receive the messages</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Consumers in a consumer group </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>share</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the consumption of messages (partitions).</t>
+    </r>
+  </si>
+  <si>
+    <t>=&gt; Only one consumer in the group consump a specific message.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What will happen if </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>quantity of consumers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the group is larger than </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>quantity of partitions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the topic?</t>
+    </r>
+  </si>
+  <si>
+    <t>=&gt; Idle consumers in the group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1947,6 +2379,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1975,7 +2415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1993,6 +2433,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2017,6 +2459,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>403412</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>187700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{843248A4-0E29-4BE2-A8E8-81E4983F7F79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7440706" y="190500"/>
+          <a:ext cx="1008530" cy="1521200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2065,7 +2556,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2378,7 +2869,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2600,10 +3091,362 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>560294</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>1631</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79ABDE50-24A2-EEDF-7ADC-7C13D6CAFAC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656294" y="15251207"/>
+          <a:ext cx="3585882" cy="1525630"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>347460</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>11206</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3038D645-FEC9-75A7-898E-0ADE1CDC5E97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656294" y="19061207"/>
+          <a:ext cx="6398637" cy="2487705"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>605117</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>403411</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>174008</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B46327A1-AA55-08D9-932B-582370CA3CFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656293" y="21929912"/>
+          <a:ext cx="5244353" cy="2650508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>31484</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6AF0439-C61F-4098-B172-BE32448899C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656294" y="16965706"/>
+          <a:ext cx="4267308" cy="1479177"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>145487</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88A80CE1-2836-15B4-E5F5-B1FCB4748218}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656294" y="25157206"/>
+          <a:ext cx="4807324" cy="3955487"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>364176</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>7389</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58CBEF91-D93D-B2CB-94ED-338163595C68}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656294" y="29359412"/>
+          <a:ext cx="4600000" cy="3638095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>287274</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>152095</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2037F5E2-E7B4-C9BF-9C5C-2051883B33D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656294" y="33561618"/>
+          <a:ext cx="5733333" cy="2438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>190</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>601560</xdr:colOff>
+      <xdr:row>206</xdr:row>
+      <xdr:rowOff>94857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74736A37-5510-3C3D-1BC3-90430ABCF990}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656294" y="36228618"/>
+          <a:ext cx="6047619" cy="3142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2658,7 +3501,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2707,63 +3550,19 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>324971</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>174517</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5399AE5-1CD7-44BA-953B-C3FAA22BA6EA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6656294" y="2868706"/>
-          <a:ext cx="5771030" cy="2460517"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>38233</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>28429</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2780,7 +3579,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2801,13 +3600,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>57280</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>18905</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2824,7 +3623,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2845,13 +3644,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>238232</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>180810</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2868,7 +3667,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2885,10 +3684,367 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>324971</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>163311</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E9DD679-E088-4FFE-BB17-63562EFA3BB0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6656294" y="2868706"/>
+          <a:ext cx="5771030" cy="2460517"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>397866</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69718E5E-ECBD-4181-A499-98A8CA38ABA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4235824" y="4964206"/>
+          <a:ext cx="4028571" cy="733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>487986</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>66548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9260D159-5553-7D46-D4A8-540CE810A62C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4235824" y="5916706"/>
+          <a:ext cx="4723809" cy="1019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>497510</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>57048</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F483A4AE-E1C2-A49E-13AF-77070BEFB4D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4235824" y="7250206"/>
+          <a:ext cx="4733333" cy="819048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>487986</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>133262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF3E9F90-BD66-4FAD-9C7A-87E7DCB1D597}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4235824" y="8202706"/>
+          <a:ext cx="4723809" cy="704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>177532</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>28429</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92A925D6-ADA1-45F0-739E-7D4741D11636}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1210235" y="12584206"/>
+          <a:ext cx="14095238" cy="1171429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>158484</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>47476</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4496675-4C7B-CB94-C528-8312D5CFC3FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1210235" y="16775206"/>
+          <a:ext cx="14076190" cy="1190476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>177532</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>57000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23829B86-63B1-4A81-4FEB-E599939C2A22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1210235" y="18489706"/>
+          <a:ext cx="14095238" cy="1200000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3246,13 +4402,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
@@ -3350,6 +4507,9 @@
       <c r="I11" s="5" t="s">
         <v>36</v>
       </c>
+      <c r="J11" s="4">
+        <v>45029</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -3403,6 +4563,9 @@
       <c r="I15" s="5" t="s">
         <v>291</v>
       </c>
+      <c r="J15" s="4">
+        <v>45030</v>
+      </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -3426,7 +4589,7 @@
         <v>21</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -3437,7 +4600,7 @@
         <v>22</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -3448,7 +4611,7 @@
         <v>23</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -3457,7 +4620,7 @@
     <hyperlink ref="B3" r:id="rId1" xr:uid="{861A99EE-0921-421F-BC96-900791BB5872}"/>
     <hyperlink ref="I6" location="'S1'!A1" display="S1" xr:uid="{3D87809D-6E45-43CE-9725-A548423AA037}"/>
     <hyperlink ref="I7" location="'S1'!A1" display="S1" xr:uid="{4282C628-6489-4003-ACD2-BB66DA487B4D}"/>
-    <hyperlink ref="I11" location="'S5'!A1" display="'S5" xr:uid="{A2B08A41-5AA0-48D0-A518-FE6A82B637CB}"/>
+    <hyperlink ref="I11" location="S5.Kafka!A1" display="S5" xr:uid="{A2B08A41-5AA0-48D0-A518-FE6A82B637CB}"/>
     <hyperlink ref="I8" location="'S2-S4'!A1" display="'S2-S4" xr:uid="{52A293F6-3EB0-40CE-B160-67F43641EAD7}"/>
     <hyperlink ref="I9" location="'S2-S4'!A80" display="S2-S4" xr:uid="{B8F8482C-5365-4C8D-9F18-0955EF82A074}"/>
     <hyperlink ref="I10" location="'S2-S4'!A110" display="S2-S4" xr:uid="{82B3C322-8008-4D18-88CB-A3A1339B1A3F}"/>
@@ -3472,6 +4635,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3566,7 +4730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5AB75A-A144-41A1-81E4-EBE7D4C71C13}">
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I81" sqref="I81"/>
     </sheetView>
   </sheetViews>
@@ -3867,7 +5031,7 @@
         <v>81</v>
       </c>
       <c r="H69" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="70" spans="4:8" x14ac:dyDescent="0.25">
@@ -3875,7 +5039,7 @@
         <v>82</v>
       </c>
       <c r="H70" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="71" spans="4:8" x14ac:dyDescent="0.25">
@@ -3888,7 +5052,7 @@
         <v>84</v>
       </c>
       <c r="H72" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="73" spans="4:8" x14ac:dyDescent="0.25">
@@ -3946,7 +5110,7 @@
         <v>95</v>
       </c>
       <c r="H83" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="84" spans="4:8" x14ac:dyDescent="0.25">
@@ -4105,7 +5269,7 @@
         <v>123</v>
       </c>
       <c r="H111" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="112" spans="3:8" x14ac:dyDescent="0.25">
@@ -4123,7 +5287,7 @@
         <v>126</v>
       </c>
       <c r="H114" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="115" spans="4:8" x14ac:dyDescent="0.25">
@@ -4131,15 +5295,15 @@
         <v>127</v>
       </c>
       <c r="H115" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="116" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D116" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="H116" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="117" spans="4:8" x14ac:dyDescent="0.25">
@@ -4176,7 +5340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BEC7585-FE2F-4A40-88C4-78CA0BE05EE9}">
   <dimension ref="A1:G172"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
@@ -4739,7 +5903,7 @@
     </row>
     <row r="151" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C151" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.25">
@@ -4794,10 +5958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B2B8F6-45D6-4830-9424-A9D0AFC17EA2}">
-  <dimension ref="A1:J81"/>
+  <dimension ref="A1:J200"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G82" sqref="G82"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4822,12 +5986,12 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>293</v>
+        <v>483</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>294</v>
+        <v>508</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4914,7 +6078,7 @@
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="C38" s="11" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5028,9 +6192,254 @@
         <v>285</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="10" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="2" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B100" s="17" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D102" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D103" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D104" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D105" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C108" s="10" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D109" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C116" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D117" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E118" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="119" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D119" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="121" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D121" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="123" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D123" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E124" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="125" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E125" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="126" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D126" s="8" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="127" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D127" s="8" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="133" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D133" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E134" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="135" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D135" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="137" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D137" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="154" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B154" s="17" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C155" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C156" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C158" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D159" s="6" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C160" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D161" s="6" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B175" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C176" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B190" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C191" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D192" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="194" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C194" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="195" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C195" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="196" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D196" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="198" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C198" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="199" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D199" s="6" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="200" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D200" t="s">
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -5061,17 +6470,17 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -5084,52 +6493,52 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -5139,7 +6548,7 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -5172,35 +6581,35 @@
         <v>197</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D30" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D31" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E32" s="12" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E33" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E34" s="12" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -5215,38 +6624,38 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D43" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C44" s="16" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D44" s="6"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -5261,15 +6670,15 @@
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C50" s="8" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C51" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
@@ -5279,7 +6688,7 @@
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
@@ -5289,38 +6698,38 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C57" s="10" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C59" s="10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C61" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.25">
@@ -5330,55 +6739,55 @@
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C69" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="78" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -5395,8 +6804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E487DA4-10ED-47E3-A05C-4D73F3D4F01D}">
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71:C73"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5416,74 +6825,74 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D19" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D20" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D21" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C22" s="6" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C23" s="6"/>
       <c r="D23" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="L23" s="9" t="s">
         <v>351</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="L23" s="9" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
@@ -5491,32 +6900,32 @@
         <v>135</v>
       </c>
       <c r="H24" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L24" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H25" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H26" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L26" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
@@ -5531,42 +6940,42 @@
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -5581,7 +6990,7 @@
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C43" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -5596,50 +7005,50 @@
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C46" s="8" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C47" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C49" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C50" s="6"/>
       <c r="D50" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="G50" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="G50" s="9" t="s">
-        <v>382</v>
-      </c>
       <c r="J50" s="9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C51" s="6"/>
       <c r="D51" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="G51" t="s">
+        <v>383</v>
+      </c>
+      <c r="J51" t="s">
         <v>385</v>
-      </c>
-      <c r="J51" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C52" s="6"/>
       <c r="G52" t="s">
+        <v>384</v>
+      </c>
+      <c r="J52" t="s">
         <v>386</v>
-      </c>
-      <c r="J52" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -5654,7 +7063,7 @@
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C56" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -5674,7 +7083,7 @@
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C61" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
@@ -5684,7 +7093,7 @@
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C63" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -5699,12 +7108,12 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C67" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C68" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
@@ -5719,12 +7128,12 @@
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -5739,10 +7148,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A936B69-2286-415C-A850-753FCE73A0A6}">
-  <dimension ref="A1:L83"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5753,8 +7162,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>397</v>
+      <c r="B2" s="10" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -5767,234 +7176,242 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="L15" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>341</v>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="17" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>161</v>
+      <c r="C18" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>311</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>358</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>359</v>
+      <c r="B22" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>198</v>
+      <c r="C24" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="6" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C27" s="6" t="s">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="6" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="6" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="8" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C29" s="8" t="s">
-        <v>398</v>
-      </c>
-    </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C30" s="6" t="s">
-        <v>413</v>
+      <c r="C30" s="8" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="8" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="11" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="6" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="11" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C41" s="6"/>
-    </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C42" s="6"/>
+      <c r="C42" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C43" s="6"/>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>405</v>
-      </c>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="6"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C45" s="6"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>406</v>
+      <c r="C51" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>407</v>
+      <c r="B52" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C53" t="s">
-        <v>408</v>
+      <c r="B53" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>409</v>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="15" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D58" s="15" t="s">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
         <v>417</v>
-      </c>
-    </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D77" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D78" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D82" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D83" t="s">
-        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -6009,10 +7426,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3045F74-1FEA-4B60-9880-06E29355AB50}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6024,7 +7441,17 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>454</v>
+        <v>451</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -6037,27 +7464,332 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>458</v>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="6" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="8" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="6" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="6" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="6" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="6" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="6" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="6" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="6" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="6" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="6" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="6" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="6" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="6"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="6"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="6"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="6" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="6" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="6" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="18" t="s">
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -6065,6 +7797,8 @@
     <hyperlink ref="A1" location="Intro!A1" display="Intro" xr:uid="{33E6450B-1BD5-46E9-9440-5BF0A52E70D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6073,7 +7807,7 @@
   <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6093,12 +7827,12 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -6113,22 +7847,22 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -6153,17 +7887,17 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" s="6" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -6178,71 +7912,71 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C36" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>431</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="6" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" s="6" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C40" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
@@ -6252,37 +7986,37 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C52" s="6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C53" s="6" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C61" s="11" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -6297,12 +8031,12 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C67" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C68" s="6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -6312,12 +8046,12 @@
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
@@ -6332,12 +8066,12 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
@@ -6347,12 +8081,12 @@
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C79" s="6" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C80" s="6" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kafka: basic course 2/2 (completed)
</commit_message>
<xml_diff>
--- a/202304_Kafka/202304_Kafka.xlsx
+++ b/202304_Kafka/202304_Kafka.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\202304_Kafka\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF507B5A-46AB-47A4-A683-D2C9B43868D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFED5C0C-A941-4850-9010-7335DDF60318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,9 @@
     <sheet name="S8" sheetId="8" r:id="rId7"/>
     <sheet name="S9" sheetId="9" r:id="rId8"/>
     <sheet name="S10" sheetId="10" r:id="rId9"/>
-    <sheet name="S11" sheetId="11" r:id="rId10"/>
-    <sheet name="S12" sheetId="12" r:id="rId11"/>
-    <sheet name="S13" sheetId="13" r:id="rId12"/>
+    <sheet name="S11.Java" sheetId="11" r:id="rId10"/>
+    <sheet name="S12.Node" sheetId="12" r:id="rId11"/>
+    <sheet name="S13.Python" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="681">
   <si>
     <t>https://www.udemy.com/course/apache_kafka/</t>
   </si>
@@ -1545,13 +1545,7 @@
     <t>GET INFORMATION FROM ZOOKEEPER ABOUT ACTIVE BROKER IDS</t>
   </si>
   <si>
-    <t>bin/zookeeper-shell.sh localhost:2181 ls /brokers/ids</t>
-  </si>
-  <si>
     <t>GET INFORMATION FROM ZOOKEEPER ABOUT SPECIFIC BROKER BY ID</t>
-  </si>
-  <si>
-    <t>bin/zookeeper-shell.sh localhost:2181 get /brokers/ids/0</t>
   </si>
   <si>
     <t>--bootstrap-server localhost:9092,localhost:9093,localhost:9094 \</t>
@@ -2265,6 +2259,747 @@
   </si>
   <si>
     <t>=&gt; Idle consumers in the group</t>
+  </si>
+  <si>
+    <t>Create NodeJS producer and consumer</t>
+  </si>
+  <si>
+    <t>Init NodeJS project</t>
+  </si>
+  <si>
+    <t>npm init</t>
+  </si>
+  <si>
+    <t>npm install --save kafkajs</t>
+  </si>
+  <si>
+    <t>node producer.js</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "level": "ERROR",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "timestamp": "2023-04-15T01:14:30.650Z",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "logger": "kafkajs",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "message": "[Connection] Response Metadata(key: 3, version: 6)",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "broker": "localhost:9092",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "clientId": "tung-app",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "error": "There is no leader for this topic-partition as we are in the middle of a leadership election",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "correlationId": 1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  "size": 210</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>Kafka cluster with multiple brokers: different broker id, port, log directory.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bin/zookeeper-shell.sh localhost:2181 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /brokers/ids</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">bin/zookeeper-shell.sh localhost:2181 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> /brokers/ids/0</t>
+    </r>
+  </si>
+  <si>
+    <t>--topic cars \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  clientId: 'tung-producer',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  brokers: ['localhost:9092', 'localhost:9093'],</t>
+  </si>
+  <si>
+    <t>});</t>
+  </si>
+  <si>
+    <t>const run = async () =&gt; {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    topic: 'tung-topic',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    messages: [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      { value: 'Hi Kafka!' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      { value: 'My name is Tung.' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      { value: 'Nice to meet you.' },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  });</t>
+  </si>
+  <si>
+    <t>};</t>
+  </si>
+  <si>
+    <t>run().catch(console.error);</t>
+  </si>
+  <si>
+    <t>producer.js</t>
+  </si>
+  <si>
+    <t>Produce random animal names</t>
+  </si>
+  <si>
+    <t>npm install --save chance</t>
+  </si>
+  <si>
+    <t>const { Chance } = require('chance');</t>
+  </si>
+  <si>
+    <t>const chance = new Chance();</t>
+  </si>
+  <si>
+    <t>const value = chance.animal();</t>
+  </si>
+  <si>
+    <t>// Generate random animal</t>
+  </si>
+  <si>
+    <r>
+      <t>const { Kafka } = require('</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>kafkajs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>');</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const kafka = new </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kafka</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>({</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  await producer.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>connect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  await producer.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>send</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>({</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>const producer = kafka.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>producer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <t>Create Consumer</t>
+  </si>
+  <si>
+    <t>Create Producer</t>
+  </si>
+  <si>
+    <t>Start up Kafka cluster with 2 brokers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  clientId: 'tung-consumer',</t>
+  </si>
+  <si>
+    <t>const consumer = kafka.consumer({ groupId: 'consumer-group' });</t>
+  </si>
+  <si>
+    <t>const topic = 'animals';</t>
+  </si>
+  <si>
+    <t>consumer.js</t>
+  </si>
+  <si>
+    <t>--replication-factor 2 \</t>
+  </si>
+  <si>
+    <t>Create Python producer and consumer</t>
+  </si>
+  <si>
+    <t>Init project</t>
+  </si>
+  <si>
+    <t>Download Python 2.x or 3.x</t>
+  </si>
+  <si>
+    <t>Launch Python producer</t>
+  </si>
+  <si>
+    <t>sudo pip install kafka-python</t>
+  </si>
+  <si>
+    <t>sudo pip3 install kafka-python</t>
+  </si>
+  <si>
+    <t>producer.py</t>
+  </si>
+  <si>
+    <t>python3 producer.py</t>
+  </si>
+  <si>
+    <t>Launch Python consumer</t>
+  </si>
+  <si>
+    <t>consumer.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  'test',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  bootstrap_servers=['localhost:9092', 'localhost:9093'],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  group_id='test-consumer-group'</t>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>for message in consumer:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  print(message);</t>
+  </si>
+  <si>
+    <t>import time;</t>
+  </si>
+  <si>
+    <t>time.sleep(20);</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from kafka import </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KafkaProducer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">producer = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KafkaProducer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bootstrap_servers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=['localhost:9092', 'localhost:9093']);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>producer.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>send</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>('test', b'Hello from Tung');</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">from kafka import </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KafkaConsumer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">consumer = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>KafkaConsumer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+  </si>
+  <si>
+    <t>python3 consumer.py</t>
+  </si>
+  <si>
+    <t>Generate fake names in the messages</t>
+  </si>
+  <si>
+    <t>sudo pip install Faker</t>
+  </si>
+  <si>
+    <t>Create Java producer and consumer</t>
+  </si>
+  <si>
+    <t>Install IntelliJ</t>
+  </si>
+  <si>
+    <t>Configure Maven project</t>
+  </si>
+  <si>
+    <t>https://kafka.apache.org/documentation/</t>
+  </si>
+  <si>
+    <t>Explain Producer parameters</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1 (default)</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>https://kafka.apache.org/documentation/#producerconfigs</t>
+  </si>
+  <si>
+    <t>key.serializer</t>
+  </si>
+  <si>
+    <t>value.serializer</t>
+  </si>
+  <si>
+    <t>ack</t>
+  </si>
+  <si>
+    <t>which serializer interface to use to encode (StringSerializer, IntegerSerializer)</t>
+  </si>
+  <si>
+    <t>bootstrap.servers</t>
+  </si>
+  <si>
+    <t>producer not wait for any ack</t>
+  </si>
+  <si>
+    <t>buffer.memory</t>
+  </si>
+  <si>
+    <t>compression.type</t>
+  </si>
+  <si>
+    <t>only wait for ack from leader</t>
+  </si>
+  <si>
+    <t>wait for acks from leader and all followers.</t>
+  </si>
+  <si>
+    <t>batch.size</t>
+  </si>
+  <si>
+    <t>32 MB</t>
+  </si>
+  <si>
+    <t>total bytes of memory used to buffer records waiting to be sent to the server</t>
+  </si>
+  <si>
+    <t>none / gzip / …</t>
+  </si>
+  <si>
+    <t>the compression type for all data generated by producer</t>
+  </si>
+  <si>
+    <t>retries</t>
+  </si>
+  <si>
+    <t>resend any record whose send fails</t>
+  </si>
+  <si>
+    <t>0 / 1 / …</t>
+  </si>
+  <si>
+    <t>ssl.key.password</t>
+  </si>
+  <si>
+    <t>the password of the private key in the key store file</t>
+  </si>
+  <si>
+    <t>ssl.keystore.location</t>
+  </si>
+  <si>
+    <t>combine records into the fewer requests increasing throughput but may be latency</t>
+  </si>
+  <si>
+    <t>16384</t>
+  </si>
+  <si>
+    <t>Explain Consumer parameters</t>
+  </si>
+  <si>
+    <t>localhost:9092; …</t>
+  </si>
+  <si>
+    <t>client.id</t>
+  </si>
+  <si>
+    <t>custom id of producer</t>
+  </si>
+  <si>
+    <t>https://kafka.apache.org/documentation/#consumerconfigs</t>
+  </si>
+  <si>
+    <t>key.deserializer</t>
+  </si>
+  <si>
+    <t>value.deserializer</t>
+  </si>
+  <si>
+    <t>which serializer interface to use to decode (StringSerializer, IntegerSerializer)</t>
+  </si>
+  <si>
+    <t>Consumer with Manual-committing</t>
+  </si>
+  <si>
+    <t>Consumer with Auto-committing</t>
+  </si>
+  <si>
+    <t>Producer parameters / Consumer parameters</t>
+  </si>
+  <si>
+    <t>Consumer with Auto-committing / Manual-committing</t>
+  </si>
+  <si>
+    <t>Enable manual committing and send confirmation to brokers only when all operations successfully completed.</t>
+  </si>
+  <si>
+    <t>E.g., insert to DB</t>
+  </si>
+  <si>
+    <t>group.id</t>
+  </si>
+  <si>
+    <t>enable.auto.commit</t>
+  </si>
+  <si>
+    <t>auto.commit.interval.ms</t>
+  </si>
+  <si>
+    <t>consumer group id</t>
+  </si>
+  <si>
+    <t>enable.auto.commit = true</t>
+  </si>
+  <si>
+    <t>auto.commit.interval.ms = 1000</t>
+  </si>
+  <si>
+    <t>ConsumerRecords&lt;String, String&gt; records = consumer.poll(Duration.ofMillis(100));</t>
+  </si>
+  <si>
+    <t>// Pull records every 100ms</t>
+  </si>
+  <si>
+    <t>Set props:</t>
+  </si>
+  <si>
+    <t>for (ConsumerRecords&lt;String, String&gt; record: records) {</t>
+  </si>
+  <si>
+    <t>record.offset(), record.partition(), record.key(), record.value()</t>
+  </si>
+  <si>
+    <t>NOTE: messages are consumed by batch</t>
+  </si>
+  <si>
+    <t>auto committing</t>
+  </si>
+  <si>
+    <t>heartbeat.interval.ms</t>
+  </si>
+  <si>
+    <t>customer is alive</t>
+  </si>
+  <si>
+    <t>3000ms</t>
+  </si>
+  <si>
+    <t>session.timeout.ms</t>
+  </si>
+  <si>
+    <t>10000ms</t>
+  </si>
+  <si>
+    <t>3 heart beat</t>
+  </si>
+  <si>
+    <t>ssl.keystore.password</t>
+  </si>
+  <si>
+    <t>enable.auto.commit = false</t>
+  </si>
+  <si>
+    <t>Consumer with Partitions Assignment</t>
+  </si>
+  <si>
+    <t>Launch multiple consumers in the same consumer group</t>
   </si>
 </sst>
 </file>
@@ -2415,7 +3150,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2435,6 +3170,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2496,6 +3232,143 @@
         <a:xfrm>
           <a:off x="7440706" y="190500"/>
           <a:ext cx="1008530" cy="1521200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>230843</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>180833</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0788449-C9D0-4892-AA63-6532F6E27486}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="12203206"/>
+          <a:ext cx="4466667" cy="1133333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>523235</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>171357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9A02222-82A0-0AC3-299B-74E200C8C7F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1210235" y="13346206"/>
+          <a:ext cx="9600000" cy="742857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>86562</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AED789C4-160D-A1BC-F7E6-7BA57CB65770}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="3630706"/>
+          <a:ext cx="6742857" cy="2809524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3547,6 +4420,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>129775</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EEA9A54-4EE0-951A-3784-4C66AD389C10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6051176" y="7059706"/>
+          <a:ext cx="6180952" cy="800000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4403,7 +5320,7 @@
   <dimension ref="B2:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4581,7 +5498,7 @@
         <v>45022</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -4589,10 +5506,13 @@
         <v>21</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+      <c r="J17" s="4">
+        <v>45032</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>33</v>
       </c>
@@ -4600,10 +5520,13 @@
         <v>22</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+      <c r="J18" s="4">
+        <v>45031</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -4611,7 +5534,10 @@
         <v>23</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
+      </c>
+      <c r="J19" s="4">
+        <v>45031</v>
       </c>
     </row>
   </sheetData>
@@ -4629,9 +5555,9 @@
     <hyperlink ref="I14" location="'S8'!A1" display="'S8" xr:uid="{C343E875-D148-45C4-B77B-65AE48E324D7}"/>
     <hyperlink ref="I15" location="'S9'!A1" display="'S9" xr:uid="{F5C7CD4E-E67C-4BE2-98FC-D4B794DDBF32}"/>
     <hyperlink ref="I16" location="'S10'!A1" display="'S10" xr:uid="{0AB7EA9D-6E0B-45FA-97F5-9C4399FAC9BD}"/>
-    <hyperlink ref="I17" location="'S11'!A1" display="S11" xr:uid="{C710A1F0-4892-400D-A6F3-C2D8239ACAE3}"/>
-    <hyperlink ref="I18" location="'S12'!A1" display="'S12" xr:uid="{D9177FB2-C905-4FAB-BCBE-EA17B685743C}"/>
-    <hyperlink ref="I19" location="'S13'!A1" display="'S13" xr:uid="{93ADFB05-EA21-4FE9-B722-9646DF7D2621}"/>
+    <hyperlink ref="I17" location="S11.Java!A1" display="S11" xr:uid="{C710A1F0-4892-400D-A6F3-C2D8239ACAE3}"/>
+    <hyperlink ref="I18" location="S12.Node!A1" display="S12" xr:uid="{D9177FB2-C905-4FAB-BCBE-EA17B685743C}"/>
+    <hyperlink ref="I19" location="S13.Python!A1" display="S13" xr:uid="{93ADFB05-EA21-4FE9-B722-9646DF7D2621}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4641,52 +5567,770 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAF9745-FC6D-4392-A855-A2758A6787BD}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>612</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>621</v>
+      </c>
+      <c r="F16" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>625</v>
+      </c>
+      <c r="F18" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="F20" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="F21" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="F22" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>632</v>
+      </c>
+      <c r="F24" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>634</v>
+      </c>
+      <c r="F26" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="F28" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>638</v>
+      </c>
+      <c r="F30" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>649</v>
+      </c>
+      <c r="F41" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>625</v>
+      </c>
+      <c r="F43" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>673</v>
+      </c>
+      <c r="F50" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>675</v>
+      </c>
+      <c r="F52" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C62" s="6" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="19" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C67" s="10" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="11" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>680</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="Intro!A1" display="Intro" xr:uid="{5E25DA9D-B7F5-4C21-AAEA-1AC9DB9363F3}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{8E189D0B-4736-4470-9E8A-9B8C55990F35}"/>
+    <hyperlink ref="C15" r:id="rId2" location="producerconfigs" xr:uid="{114EB221-F521-469A-9B11-1583C5D41243}"/>
+    <hyperlink ref="C40" r:id="rId3" location="consumerconfigs" xr:uid="{7E7BCF8C-E211-40B2-AB31-1D49D5586202}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE1C4B7-0CC4-493D-B9AC-46B8DA8C0C3E}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>533</v>
+      </c>
+      <c r="J2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>135</v>
+      </c>
+      <c r="H15" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>344</v>
+      </c>
+      <c r="H16" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>345</v>
+      </c>
+      <c r="H17" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D21" s="7" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="7" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="7" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="7" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D26" s="7" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D27" s="7" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D29" s="7" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D30" s="7" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D31" s="7" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D32" s="7" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="7" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="7" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D35" s="7" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D36" s="7" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="7" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D38" s="7" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="7" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D40" s="7" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D48" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D49" s="10" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D50" s="10" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D58" s="7" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D59" s="7" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D60" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="8" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="8" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="6"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="6"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C72" s="6"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D78" s="7" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D80" s="7" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" s="7" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="7" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="7" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D84" s="7"/>
+    </row>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D85" s="7" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D86" s="7" t="s">
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -4694,28 +6338,170 @@
     <hyperlink ref="A1" location="Intro!A1" display="Intro" xr:uid="{3E886460-9B30-4372-A1C6-C806112ACA6C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97FBD846-2EA6-4955-A3BB-E5F1A774022D}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>586</v>
+      </c>
+      <c r="J2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D17" s="7" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="7" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="7" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="7" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="7" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="7" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="7" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="7" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D30" s="7" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="7" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="7" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="7" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -4730,8 +6516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC5AB75A-A144-41A1-81E4-EBE7D4C71C13}">
   <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5052,7 +6838,7 @@
         <v>84</v>
       </c>
       <c r="H72" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="73" spans="4:8" x14ac:dyDescent="0.25">
@@ -5110,7 +6896,7 @@
         <v>95</v>
       </c>
       <c r="H83" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="84" spans="4:8" x14ac:dyDescent="0.25">
@@ -5961,7 +7747,7 @@
   <dimension ref="A1:J200"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5986,12 +7772,12 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -6199,247 +7985,247 @@
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D84" s="10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C86" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C90" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D91" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="100" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B100" s="17" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C101" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D104" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D105" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="108" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C108" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D109" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="116" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C116" s="2" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="117" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="118" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E118" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="119" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D119" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="121" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D121" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="123" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D123" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="124" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E124" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="125" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E125" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="126" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D126" s="8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="127" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D127" s="8" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C132" s="2" t="s">
         <v>482</v>
-      </c>
-    </row>
-    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C132" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="133" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="134" spans="3:5" x14ac:dyDescent="0.25">
       <c r="E134" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="135" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D135" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="137" spans="3:5" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="154" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B154" s="17" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="155" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C155" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="156" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C156" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="157" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="158" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="159" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D159" s="6" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="160" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D161" s="6" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="175" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B175" s="2" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="176" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C176" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="190" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="191" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C191" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="192" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D192" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="194" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C194" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="195" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C195" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="196" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D196" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="198" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C198" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="199" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D199" s="6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="200" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -6457,8 +8243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEFBFF6-A772-431B-92C5-2CC7EF1A6305}">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6802,10 +8588,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E487DA4-10ED-47E3-A05C-4D73F3D4F01D}">
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6815,6 +8601,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>549</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>28</v>
@@ -6965,175 +8756,180 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>370</v>
+        <v>550</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C43" s="6" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C44" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="6" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C45" s="8" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C46" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="6" t="s">
         <v>375</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C47" s="6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C49" s="6" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C50" s="6"/>
-      <c r="D50" s="9" t="s">
-        <v>378</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>380</v>
-      </c>
-      <c r="J50" s="9" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C51" s="6"/>
-      <c r="D51" t="s">
-        <v>382</v>
-      </c>
-      <c r="G51" t="s">
-        <v>383</v>
-      </c>
-      <c r="J51" t="s">
-        <v>385</v>
+      <c r="D51" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="J51" s="9" t="s">
+        <v>377</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C52" s="6"/>
+      <c r="D52" t="s">
+        <v>380</v>
+      </c>
       <c r="G52" t="s">
+        <v>381</v>
+      </c>
+      <c r="J52" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="6"/>
+      <c r="G53" t="s">
+        <v>382</v>
+      </c>
+      <c r="J53" t="s">
         <v>384</v>
       </c>
-      <c r="J52" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C56" s="6" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C57" s="6" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C58" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C61" s="6" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C62" s="6" t="s">
-        <v>205</v>
+        <v>371</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C63" s="6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C64" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C67" s="6" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C68" s="6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="6" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>214</v>
-      </c>
-    </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C72" s="6" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" s="6" t="s">
-        <v>381</v>
+        <v>371</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="6" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="6" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -7151,7 +8947,7 @@
   <dimension ref="A1:L85"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7163,7 +8959,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -7186,17 +8982,17 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -7204,7 +9000,7 @@
         <v>299</v>
       </c>
       <c r="L15" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -7217,7 +9013,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -7262,7 +9058,7 @@
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -7272,42 +9068,42 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" s="8" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" s="8" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C34" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C38" s="11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
@@ -7317,7 +9113,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -7331,87 +9127,87 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D60" s="15" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D79" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D80" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D84" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D85" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -7428,7 +9224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3045F74-1FEA-4B60-9880-06E29355AB50}">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -7441,17 +9237,17 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -7469,22 +9265,22 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -7519,7 +9315,7 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" s="6" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -7534,12 +9330,12 @@
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" s="8" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" s="6" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -7554,7 +9350,7 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" s="6" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -7579,12 +9375,12 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -7604,17 +9400,17 @@
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C42" s="6" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C45" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
@@ -7629,52 +9425,52 @@
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C49" s="6" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C53" s="6" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C57" s="6" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C58" s="6" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
@@ -7684,17 +9480,17 @@
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C63" s="6" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C64" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C66" s="6" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
@@ -7714,37 +9510,37 @@
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C74" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C75" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C76" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
@@ -7759,12 +9555,12 @@
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C85" s="6" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C86" s="6" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
@@ -7774,22 +9570,22 @@
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C96" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="6" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C106" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C107" s="18" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>
@@ -7832,7 +9628,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -7887,17 +9683,17 @@
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -7917,66 +9713,66 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C36" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C40" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
@@ -7986,37 +9782,37 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C52" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C53" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C61" s="11" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -8031,12 +9827,12 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C67" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C68" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -8046,12 +9842,12 @@
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
@@ -8066,12 +9862,12 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C77" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
@@ -8081,12 +9877,12 @@
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C79" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C80" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>